<commit_message>
Tabla general de piezas y planos case electroninca.
</commit_message>
<xml_diff>
--- a/Lista de piezas clasificadas.xlsx
+++ b/Lista de piezas clasificadas.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ishan\Documents\CNC-UNI-Monografia-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\CNC-UNI-Monografia-\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
-    <sheet name="Fabricacion de estructura" sheetId="1" r:id="rId1"/>
-    <sheet name="Corte de perfileria" sheetId="2" r:id="rId2"/>
-    <sheet name="Corte de lamina" sheetId="3" r:id="rId3"/>
-    <sheet name="Maquinar piezas" sheetId="4" r:id="rId4"/>
-    <sheet name="Soldadura de estructura" sheetId="5" r:id="rId5"/>
-    <sheet name="Torneado" sheetId="6" r:id="rId6"/>
-    <sheet name="Fresado" sheetId="7" r:id="rId7"/>
-    <sheet name="Taladrado" sheetId="8" r:id="rId8"/>
+    <sheet name="General" sheetId="9" r:id="rId1"/>
+    <sheet name="Fabricacion de estructura" sheetId="1" r:id="rId2"/>
+    <sheet name="Corte de perfileria" sheetId="2" r:id="rId3"/>
+    <sheet name="Corte de lamina" sheetId="3" r:id="rId4"/>
+    <sheet name="Maquinar piezas" sheetId="4" r:id="rId5"/>
+    <sheet name="Soldadura de estructura" sheetId="5" r:id="rId6"/>
+    <sheet name="Torneado" sheetId="6" r:id="rId7"/>
+    <sheet name="Fresado" sheetId="7" r:id="rId8"/>
+    <sheet name="Taladrado" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="58">
   <si>
     <t>N.º DE PIEZA</t>
   </si>
@@ -869,6 +870,76 @@
       </rPr>
       <t>lamina</t>
     </r>
+  </si>
+  <si>
+    <t>SUBENSAMBLAJE</t>
+  </si>
+  <si>
+    <t>tuerca m6</t>
+  </si>
+  <si>
+    <t>pata</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rodamiento d12 perfil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SWGDT"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>abierto</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N.º DE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="SWGDT"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>ELEMENTO</t>
+    </r>
+  </si>
+  <si>
+    <t>Solo/CANTIDAD</t>
+  </si>
+  <si>
+    <t>Marco principal</t>
+  </si>
+  <si>
+    <t>Eje Y</t>
+  </si>
+  <si>
+    <t>Eje Z</t>
+  </si>
+  <si>
+    <t>Eje X</t>
   </si>
 </sst>
 </file>
@@ -1239,6 +1310,603 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="66.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="66.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f>SUM(D2:D29)</f>
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1251,12 +1919,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,11 +2248,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1643,7 +2311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1657,7 +2325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1671,7 +2339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1734,7 +2402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1748,7 +2416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Se anexo tabla de piezas en documento acapite de manufactura
</commit_message>
<xml_diff>
--- a/Lista de piezas clasificadas.xlsx
+++ b/Lista de piezas clasificadas.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="9" r:id="rId1"/>
-    <sheet name="Fabricacion de estructura" sheetId="1" r:id="rId2"/>
-    <sheet name="Corte de perfileria" sheetId="2" r:id="rId3"/>
-    <sheet name="Corte de lamina" sheetId="3" r:id="rId4"/>
-    <sheet name="Maquinar piezas" sheetId="4" r:id="rId5"/>
-    <sheet name="Soldadura de estructura" sheetId="5" r:id="rId6"/>
-    <sheet name="Torneado" sheetId="6" r:id="rId7"/>
-    <sheet name="Fresado" sheetId="7" r:id="rId8"/>
-    <sheet name="Taladrado" sheetId="8" r:id="rId9"/>
+    <sheet name="Hoja1" sheetId="10" r:id="rId2"/>
+    <sheet name="Fabricacion de estructura" sheetId="1" r:id="rId3"/>
+    <sheet name="Corte de perfileria" sheetId="2" r:id="rId4"/>
+    <sheet name="Corte de lamina" sheetId="3" r:id="rId5"/>
+    <sheet name="Maquinar piezas" sheetId="4" r:id="rId6"/>
+    <sheet name="Soldadura de estructura" sheetId="5" r:id="rId7"/>
+    <sheet name="Torneado" sheetId="6" r:id="rId8"/>
+    <sheet name="Fresado" sheetId="7" r:id="rId9"/>
+    <sheet name="Taladrado" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="79">
   <si>
     <t>N.º DE PIEZA</t>
   </si>
@@ -904,8 +905,70 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">N.º DE </t>
+    <t>Marco principal</t>
+  </si>
+  <si>
+    <t>Eje Y</t>
+  </si>
+  <si>
+    <t>Eje Z</t>
+  </si>
+  <si>
+    <t>Eje X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">base case </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SWGDT"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>electronica</t>
+    </r>
+  </si>
+  <si>
+    <t>Inox 308L</t>
+  </si>
+  <si>
+    <t>Case superior</t>
+  </si>
+  <si>
+    <t>Lateral case superior</t>
+  </si>
+  <si>
+    <t>case panel base</t>
+  </si>
+  <si>
+    <t>case panel frontal</t>
+  </si>
+  <si>
+    <t>bisagra conjunto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Case electronica</t>
+  </si>
+  <si>
+    <t>base lateral</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lamina </t>
     </r>
     <r>
       <rPr>
@@ -923,23 +986,86 @@
         <rFont val="Century Gothic"/>
         <family val="2"/>
       </rPr>
-      <t>ELEMENTO</t>
-    </r>
-  </si>
-  <si>
-    <t>Solo/CANTIDAD</t>
-  </si>
-  <si>
-    <t>Marco principal</t>
-  </si>
-  <si>
-    <t>Eje Y</t>
-  </si>
-  <si>
-    <t>Eje Z</t>
-  </si>
-  <si>
-    <t>Eje X</t>
+      <t>espesor 4mm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">soporte angular riel </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="SWGDT"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>eje x</t>
+    </r>
+  </si>
+  <si>
+    <t>Angular 2"</t>
+  </si>
+  <si>
+    <t>Case eje Y</t>
+  </si>
+  <si>
+    <t>Taladrado</t>
+  </si>
+  <si>
+    <t>Maquinado</t>
+  </si>
+  <si>
+    <t>CNC 4.0</t>
+  </si>
+  <si>
+    <t>Soldadura</t>
+  </si>
+  <si>
+    <t>Fresado</t>
+  </si>
+  <si>
+    <r>
+      <t>base eje X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SWGDT"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>rediseñado</t>
+    </r>
+  </si>
+  <si>
+    <t>TOTAL DE PIEZAS</t>
+  </si>
+  <si>
+    <t>PROCESO DE 
+MANUFACTURA2</t>
+  </si>
+  <si>
+    <t>PROCESO DE 
+MANUFACTURA3</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1030,11 +1156,109 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1045,6 +1269,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B1:H45" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:H45"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="N.º DE PIEZA" dataDxfId="4"/>
+    <tableColumn id="2" name="SUBENSAMBLAJE" dataDxfId="3"/>
+    <tableColumn id="3" name="MATERIAL"/>
+    <tableColumn id="4" name="CANTIDAD" dataDxfId="2"/>
+    <tableColumn id="5" name="PROCESO DE _x000a_MANUFACTURA" dataDxfId="1"/>
+    <tableColumn id="6" name="PROCESO DE _x000a_MANUFACTURA2"/>
+    <tableColumn id="7" name="PROCESO DE _x000a_MANUFACTURA3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1310,602 +1550,896 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
+    <row r="1" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
+      <c r="E4" s="1">
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
+      <c r="E5" s="1">
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>5</v>
+      <c r="E7" s="1">
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
+      <c r="E8" s="1">
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1">
         <v>4</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1">
         <v>4</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
+      <c r="E12" s="1">
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="1">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="F37" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="1" t="s">
+    </row>
+    <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>4</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="66.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>2</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>3</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>5</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="66.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D30">
-        <f>SUM(D2:D29)</f>
-        <v>51</v>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45">
+        <f>SUM(E2:E44)</f>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1919,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -2248,7 +2782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2311,7 +2845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2325,7 +2859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2339,7 +2873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2402,7 +2936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2414,18 +2948,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>